<commit_message>
doc(): sprint planning y MVP inicial
</commit_message>
<xml_diff>
--- a/iteración-3/resources/Planning.xlsx
+++ b/iteración-3/resources/Planning.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>Story Points (1, 2, 3, 5, 8, 13)</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Ver ranking de la penca</t>
   </si>
   <si>
-    <t>Envìo de invitaciones para sumarse a la penca</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ver partidos del día </t>
   </si>
   <si>
@@ -142,6 +139,9 @@
   </si>
   <si>
     <t>Story Points (0, 1, 2, 3, 5, 8, 13)</t>
+  </si>
+  <si>
+    <t>Envío de invitaciones para sumarse a la penca</t>
   </si>
 </sst>
 </file>
@@ -280,11 +280,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,15 +602,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="B2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -637,13 +637,13 @@
       <c r="H3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="8" t="s">
-        <v>35</v>
+      <c r="J3" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -656,7 +656,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -669,7 +669,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -682,7 +682,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -695,7 +695,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -708,7 +708,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -721,7 +721,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -733,8 +733,8 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>23</v>
+      <c r="A11" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -746,8 +746,8 @@
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>24</v>
+      <c r="A12" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -759,8 +759,8 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>25</v>
+      <c r="A13" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -772,8 +772,8 @@
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>26</v>
+      <c r="A14" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -785,8 +785,8 @@
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>27</v>
+      <c r="A15" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -798,8 +798,8 @@
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>28</v>
+      <c r="A16" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -811,8 +811,8 @@
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>29</v>
+      <c r="A17" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -824,8 +824,8 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>30</v>
+      <c r="A18" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -837,8 +837,8 @@
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>31</v>
+      <c r="A19" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -850,8 +850,8 @@
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>32</v>
+      <c r="A20" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -863,8 +863,8 @@
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>33</v>
+      <c r="A21" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -876,8 +876,8 @@
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>34</v>
+      <c r="A22" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -898,10 +898,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,20 +909,21 @@
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -947,16 +948,19 @@
       <c r="H2" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2">
         <v>8</v>
@@ -965,33 +969,36 @@
         <v>8</v>
       </c>
       <c r="F3" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G3" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H3" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
       </c>
       <c r="D4" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E4" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F4" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G4" s="1">
         <v>5</v>
@@ -999,8 +1006,11 @@
       <c r="H4" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1008,53 +1018,59 @@
         <v>5</v>
       </c>
       <c r="C5" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F5" s="1">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G5" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H5" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="J5" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1">
         <v>3</v>
       </c>
       <c r="D6" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E6" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F6" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G6" s="1">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="H6" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="J6" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="B7" s="1">
         <v>3</v>
@@ -1063,71 +1079,80 @@
         <v>5</v>
       </c>
       <c r="D7" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E7" s="1">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F7" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H7" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="J7" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1">
+        <v>8</v>
+      </c>
+      <c r="F8" s="1">
+        <v>8</v>
+      </c>
+      <c r="G8" s="1">
+        <v>13</v>
+      </c>
+      <c r="H8" s="1">
+        <v>5</v>
+      </c>
+      <c r="J8" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1">
-        <v>2</v>
-      </c>
-      <c r="C8" s="1">
+      <c r="B9" s="1">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1">
         <v>3</v>
       </c>
-      <c r="D8" s="1">
-        <v>5</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="H9" s="1">
         <v>3</v>
       </c>
-      <c r="F8" s="1">
-        <v>3</v>
-      </c>
-      <c r="G8" s="1">
-        <v>3</v>
-      </c>
-      <c r="H8" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1">
-        <v>2</v>
-      </c>
-      <c r="H9" s="1">
-        <v>1</v>
+      <c r="J9" s="1">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>